<commit_message>
Ajout de nouveau scénarios
</commit_message>
<xml_diff>
--- a/Doc/Use Case & Scenario.xlsx
+++ b/Doc/Use Case & Scenario.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="39">
   <si>
     <t>Identifiant</t>
   </si>
@@ -109,6 +109,33 @@
   </si>
   <si>
     <t>le programme vérifie que</t>
+  </si>
+  <si>
+    <t>3-Menu</t>
+  </si>
+  <si>
+    <t>Me déplacer dans le menu</t>
+  </si>
+  <si>
+    <t>Choisir l'option voulue</t>
+  </si>
+  <si>
+    <t>si aucune option n'est sélectionnée</t>
+  </si>
+  <si>
+    <t>si l'option n'éxiste pas</t>
+  </si>
+  <si>
+    <t>si l'entrée ne correspond pas à ce qui est demandé</t>
+  </si>
+  <si>
+    <t>Redemande l'option voulue</t>
+  </si>
+  <si>
+    <t>Si l'option choisie existe</t>
+  </si>
+  <si>
+    <t>Déplace le joueur dans l'option demandée.</t>
   </si>
 </sst>
 </file>
@@ -144,7 +171,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="44">
     <border>
       <left/>
       <right/>
@@ -363,11 +390,329 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -432,6 +777,114 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -713,10 +1166,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:P32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11:P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -729,7 +1182,7 @@
     <col min="7" max="7" width="27.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -744,8 +1197,17 @@
         <v>21</v>
       </c>
       <c r="G1" s="1"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I1" s="43" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" s="46"/>
+      <c r="K1" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1" s="37"/>
+      <c r="M1" s="33"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>1</v>
       </c>
@@ -758,8 +1220,17 @@
       <c r="F2" s="15" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I2" s="44" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" s="39"/>
+      <c r="K2" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="L2" s="36"/>
+      <c r="M2" s="34"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>2</v>
       </c>
@@ -772,8 +1243,17 @@
       <c r="F3" s="15" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I3" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="39"/>
+      <c r="K3" s="41" t="s">
+        <v>31</v>
+      </c>
+      <c r="L3" s="36"/>
+      <c r="M3" s="34"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>3</v>
       </c>
@@ -786,8 +1266,17 @@
       <c r="F4" s="15" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I4" s="44" t="s">
+        <v>3</v>
+      </c>
+      <c r="J4" s="39"/>
+      <c r="K4" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="L4" s="36"/>
+      <c r="M4" s="34"/>
+    </row>
+    <row r="5" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
         <v>4</v>
       </c>
@@ -800,9 +1289,18 @@
       <c r="F5" s="16" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I5" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="J5" s="47"/>
+      <c r="K5" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="L5" s="38"/>
+      <c r="M5" s="35"/>
+    </row>
+    <row r="6" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
         <v>5</v>
       </c>
@@ -821,8 +1319,22 @@
       <c r="G7" s="10" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="I7" s="48" t="s">
+        <v>5</v>
+      </c>
+      <c r="J7" s="49"/>
+      <c r="K7" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="L7" s="49"/>
+      <c r="M7" s="49"/>
+      <c r="N7" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="O7" s="49"/>
+      <c r="P7" s="50"/>
+    </row>
+    <row r="8" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="25" t="s">
         <v>13</v>
       </c>
@@ -841,8 +1353,22 @@
       <c r="G8" s="31" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I8" s="64" t="s">
+        <v>32</v>
+      </c>
+      <c r="J8" s="65"/>
+      <c r="K8" s="52" t="s">
+        <v>33</v>
+      </c>
+      <c r="L8" s="53"/>
+      <c r="M8" s="51"/>
+      <c r="N8" s="70" t="s">
+        <v>36</v>
+      </c>
+      <c r="O8" s="71"/>
+      <c r="P8" s="72"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="26"/>
       <c r="B9" s="17" t="s">
         <v>18</v>
@@ -855,8 +1381,18 @@
         <v>18</v>
       </c>
       <c r="G9" s="32"/>
-    </row>
-    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="I9" s="66"/>
+      <c r="J9" s="67"/>
+      <c r="K9" s="56" t="s">
+        <v>34</v>
+      </c>
+      <c r="L9" s="57"/>
+      <c r="M9" s="55"/>
+      <c r="N9" s="73"/>
+      <c r="O9" s="74"/>
+      <c r="P9" s="75"/>
+    </row>
+    <row r="10" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="26"/>
       <c r="B10" s="17" t="s">
         <v>14</v>
@@ -871,8 +1407,18 @@
       <c r="G10" s="18" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="I10" s="66"/>
+      <c r="J10" s="67"/>
+      <c r="K10" s="56" t="s">
+        <v>35</v>
+      </c>
+      <c r="L10" s="57"/>
+      <c r="M10" s="55"/>
+      <c r="N10" s="76"/>
+      <c r="O10" s="77"/>
+      <c r="P10" s="78"/>
+    </row>
+    <row r="11" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="27"/>
       <c r="B11" s="17" t="s">
         <v>19</v>
@@ -883,112 +1429,228 @@
       <c r="E11" s="29"/>
       <c r="F11" s="17"/>
       <c r="G11" s="21"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I11" s="68"/>
+      <c r="J11" s="69"/>
+      <c r="K11" s="56" t="s">
+        <v>37</v>
+      </c>
+      <c r="L11" s="57"/>
+      <c r="M11" s="55"/>
+      <c r="N11" s="56" t="s">
+        <v>38</v>
+      </c>
+      <c r="O11" s="57"/>
+      <c r="P11" s="58"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="2"/>
       <c r="C12" s="4"/>
       <c r="E12" s="30"/>
       <c r="F12" s="20"/>
       <c r="G12" s="21"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I12" s="54"/>
+      <c r="J12" s="55"/>
+      <c r="K12" s="56"/>
+      <c r="L12" s="57"/>
+      <c r="M12" s="55"/>
+      <c r="N12" s="56"/>
+      <c r="O12" s="57"/>
+      <c r="P12" s="58"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="2"/>
       <c r="C13" s="4"/>
       <c r="E13" s="19"/>
       <c r="F13" s="20"/>
       <c r="G13" s="21"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I13" s="54"/>
+      <c r="J13" s="55"/>
+      <c r="K13" s="56"/>
+      <c r="L13" s="57"/>
+      <c r="M13" s="55"/>
+      <c r="N13" s="56"/>
+      <c r="O13" s="57"/>
+      <c r="P13" s="58"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="2"/>
       <c r="C14" s="4"/>
       <c r="E14" s="19"/>
       <c r="F14" s="20"/>
       <c r="G14" s="21"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I14" s="54"/>
+      <c r="J14" s="55"/>
+      <c r="K14" s="56"/>
+      <c r="L14" s="57"/>
+      <c r="M14" s="55"/>
+      <c r="N14" s="56"/>
+      <c r="O14" s="57"/>
+      <c r="P14" s="58"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="2"/>
       <c r="C15" s="4"/>
       <c r="E15" s="19"/>
       <c r="F15" s="20"/>
       <c r="G15" s="21"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I15" s="54"/>
+      <c r="J15" s="55"/>
+      <c r="K15" s="56"/>
+      <c r="L15" s="57"/>
+      <c r="M15" s="55"/>
+      <c r="N15" s="56"/>
+      <c r="O15" s="57"/>
+      <c r="P15" s="58"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="2"/>
       <c r="C16" s="4"/>
       <c r="E16" s="19"/>
       <c r="F16" s="20"/>
       <c r="G16" s="21"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I16" s="54"/>
+      <c r="J16" s="55"/>
+      <c r="K16" s="56"/>
+      <c r="L16" s="57"/>
+      <c r="M16" s="55"/>
+      <c r="N16" s="56"/>
+      <c r="O16" s="57"/>
+      <c r="P16" s="58"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="2"/>
       <c r="C17" s="4"/>
       <c r="E17" s="19"/>
       <c r="F17" s="20"/>
       <c r="G17" s="21"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I17" s="54"/>
+      <c r="J17" s="55"/>
+      <c r="K17" s="56"/>
+      <c r="L17" s="57"/>
+      <c r="M17" s="55"/>
+      <c r="N17" s="56"/>
+      <c r="O17" s="57"/>
+      <c r="P17" s="58"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="2"/>
       <c r="C18" s="4"/>
       <c r="E18" s="19"/>
       <c r="F18" s="20"/>
       <c r="G18" s="21"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I18" s="54"/>
+      <c r="J18" s="55"/>
+      <c r="K18" s="56"/>
+      <c r="L18" s="57"/>
+      <c r="M18" s="55"/>
+      <c r="N18" s="56"/>
+      <c r="O18" s="57"/>
+      <c r="P18" s="58"/>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="2"/>
       <c r="C19" s="4"/>
       <c r="E19" s="19"/>
       <c r="F19" s="20"/>
       <c r="G19" s="21"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I19" s="54"/>
+      <c r="J19" s="55"/>
+      <c r="K19" s="56"/>
+      <c r="L19" s="57"/>
+      <c r="M19" s="55"/>
+      <c r="N19" s="56"/>
+      <c r="O19" s="57"/>
+      <c r="P19" s="58"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="2"/>
       <c r="C20" s="4"/>
       <c r="E20" s="19"/>
       <c r="F20" s="20"/>
       <c r="G20" s="21"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I20" s="54"/>
+      <c r="J20" s="55"/>
+      <c r="K20" s="56"/>
+      <c r="L20" s="57"/>
+      <c r="M20" s="55"/>
+      <c r="N20" s="56"/>
+      <c r="O20" s="57"/>
+      <c r="P20" s="58"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="2"/>
       <c r="C21" s="4"/>
       <c r="E21" s="19"/>
       <c r="F21" s="20"/>
       <c r="G21" s="21"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I21" s="54"/>
+      <c r="J21" s="55"/>
+      <c r="K21" s="56"/>
+      <c r="L21" s="57"/>
+      <c r="M21" s="55"/>
+      <c r="N21" s="56"/>
+      <c r="O21" s="57"/>
+      <c r="P21" s="58"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="2"/>
       <c r="C22" s="4"/>
       <c r="E22" s="19"/>
       <c r="F22" s="20"/>
       <c r="G22" s="21"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I22" s="54"/>
+      <c r="J22" s="55"/>
+      <c r="K22" s="56"/>
+      <c r="L22" s="57"/>
+      <c r="M22" s="55"/>
+      <c r="N22" s="56"/>
+      <c r="O22" s="57"/>
+      <c r="P22" s="58"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="2"/>
       <c r="C23" s="4"/>
       <c r="E23" s="19"/>
       <c r="F23" s="20"/>
       <c r="G23" s="21"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I23" s="54"/>
+      <c r="J23" s="55"/>
+      <c r="K23" s="56"/>
+      <c r="L23" s="57"/>
+      <c r="M23" s="55"/>
+      <c r="N23" s="56"/>
+      <c r="O23" s="57"/>
+      <c r="P23" s="58"/>
+    </row>
+    <row r="24" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3"/>
       <c r="B24" s="2"/>
       <c r="C24" s="4"/>
       <c r="E24" s="19"/>
       <c r="F24" s="20"/>
       <c r="G24" s="21"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I24" s="59"/>
+      <c r="J24" s="60"/>
+      <c r="K24" s="61"/>
+      <c r="L24" s="62"/>
+      <c r="M24" s="60"/>
+      <c r="N24" s="61"/>
+      <c r="O24" s="62"/>
+      <c r="P24" s="63"/>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="2"/>
       <c r="C25" s="4"/>
@@ -996,7 +1658,7 @@
       <c r="F25" s="20"/>
       <c r="G25" s="21"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="2"/>
       <c r="C26" s="4"/>
@@ -1004,7 +1666,7 @@
       <c r="F26" s="20"/>
       <c r="G26" s="21"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="2"/>
       <c r="C27" s="4"/>
@@ -1012,7 +1674,7 @@
       <c r="F27" s="20"/>
       <c r="G27" s="21"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="2"/>
       <c r="C28" s="4"/>
@@ -1020,7 +1682,7 @@
       <c r="F28" s="20"/>
       <c r="G28" s="21"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
       <c r="B29" s="2"/>
       <c r="C29" s="4"/>
@@ -1028,7 +1690,7 @@
       <c r="F29" s="20"/>
       <c r="G29" s="21"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="2"/>
       <c r="C30" s="4"/>
@@ -1036,7 +1698,7 @@
       <c r="F30" s="20"/>
       <c r="G30" s="21"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
       <c r="B31" s="2"/>
       <c r="C31" s="4"/>
@@ -1044,7 +1706,7 @@
       <c r="F31" s="20"/>
       <c r="G31" s="21"/>
     </row>
-    <row r="32" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="5"/>
       <c r="B32" s="7"/>
       <c r="C32" s="6"/>
@@ -1053,10 +1715,69 @@
       <c r="G32" s="24"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="62">
+    <mergeCell ref="N21:P21"/>
+    <mergeCell ref="N22:P22"/>
+    <mergeCell ref="N23:P23"/>
+    <mergeCell ref="N24:P24"/>
+    <mergeCell ref="N8:P10"/>
+    <mergeCell ref="I8:J11"/>
+    <mergeCell ref="K22:M22"/>
+    <mergeCell ref="K23:M23"/>
+    <mergeCell ref="K24:M24"/>
+    <mergeCell ref="N11:P11"/>
+    <mergeCell ref="N12:P12"/>
+    <mergeCell ref="N13:P13"/>
+    <mergeCell ref="N14:P14"/>
+    <mergeCell ref="N15:P15"/>
+    <mergeCell ref="N16:P16"/>
+    <mergeCell ref="N17:P17"/>
+    <mergeCell ref="N18:P18"/>
+    <mergeCell ref="N19:P19"/>
+    <mergeCell ref="N20:P20"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="K8:M8"/>
+    <mergeCell ref="K9:M9"/>
+    <mergeCell ref="K10:M10"/>
+    <mergeCell ref="K11:M11"/>
+    <mergeCell ref="K12:M12"/>
+    <mergeCell ref="K13:M13"/>
+    <mergeCell ref="K14:M14"/>
+    <mergeCell ref="K15:M15"/>
+    <mergeCell ref="K16:M16"/>
+    <mergeCell ref="K17:M17"/>
+    <mergeCell ref="K18:M18"/>
+    <mergeCell ref="K19:M19"/>
+    <mergeCell ref="K20:M20"/>
+    <mergeCell ref="K21:M21"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="N7:P7"/>
     <mergeCell ref="A8:A11"/>
     <mergeCell ref="E8:E12"/>
     <mergeCell ref="G8:G9"/>
+    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="K2:M2"/>
+    <mergeCell ref="K3:M3"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="K5:M5"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="K7:M7"/>
+    <mergeCell ref="I12:J12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="152" orientation="portrait" r:id="rId1"/>

</xml_diff>